<commit_message>
Only 3ph lines and loads in the IEEE 13-bus Test Case
</commit_message>
<xml_diff>
--- a/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
+++ b/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.0000 at 0.00</t>
+          <t>1.0000 at 0.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,41 +477,61 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>645</v>
+        <v>633</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.0000 at 0.00</t>
+          <t>0.9969 at -0.07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9998 at -121.27</t>
+          <t>0.9980 at -120.05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.0000 at 120.00</t>
+          <t>0.9973 at 119.99</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>646</v>
+        <v>634</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.0000 at 0.00</t>
+          <t>0.9724 at -0.77</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.0000 at 0.00</t>
+          <t>0.9788 at -120.55</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0000 at 0.00</t>
+          <t>0.9782 at 119.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>671</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.0011 at 0.01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.9980 at -120.01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.9973 at 119.81</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying to understand IEEE 13-bus test case results
</commit_message>
<xml_diff>
--- a/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
+++ b/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,77 +461,217 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.0000 at 0.00</t>
+          <t>1.0210 at -2.49</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1.0000 at -120.00</t>
+          <t>1.0420 at -121.72</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0000 at 120.00</t>
+          <t>1.0174 at 117.83</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.9969 at -0.07</t>
+          <t>0.0000 at 0.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9980 at -120.05</t>
+          <t>1.0371 at -122.38</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.9973 at 119.99</t>
+          <t>1.0101 at 117.40</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>634</v>
+        <v>646</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.9724 at -0.77</t>
+          <t>0.0000 at 0.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9788 at -120.55</t>
+          <t>1.0379 at -122.74</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.9782 at 119.50</t>
+          <t>1.0049 at 117.17</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>633</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.0180 at -2.55</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.0401 at -121.77</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1.0148 at 117.83</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>634</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.9940 at -3.23</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.0218 at -122.22</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.9960 at 117.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>671</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.0011 at 0.01</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.9980 at -120.01</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.9973 at 119.81</t>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1.0105 at -4.36</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.0558 at -121.54</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.9947 at 117.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>684</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1.0103 at -4.40</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.0000 at 0.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.9949 at 117.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>611</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.0000 at 0.00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.0000 at 0.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.9953 at 117.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>675</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1.0033 at -4.54</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1.0572 at -121.65</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.9918 at 117.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>680</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1.0105 at -4.36</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1.0558 at -121.54</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.9947 at 117.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>652</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1.0091 at -4.49</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.0000 at 0.00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.0000 at 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
IEEE 13-bus working considering all loads as impedance.
</commit_message>
<xml_diff>
--- a/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
+++ b/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0371 at -122.38</t>
+          <t>1.0389 at -121.85</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.0101 at 117.40</t>
+          <t>1.0140 at 117.90</t>
         </is>
       </c>
     </row>
@@ -506,12 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0379 at -122.74</t>
+          <t>1.0372 at -121.92</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.0049 at 117.17</t>
+          <t>1.0119 at 117.95</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.0180 at -2.55</t>
+          <t>1.0209 at -2.49</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0401 at -121.77</t>
+          <t>1.0419 at -121.72</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.0148 at 117.83</t>
+          <t>1.0173 at 117.83</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.9940 at -3.23</t>
+          <t>1.0202 at -2.51</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0218 at -122.22</t>
+          <t>1.0414 at -121.73</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.9960 at 117.35</t>
+          <t>1.0168 at 117.82</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.0121 at -4.75</t>
+          <t>1.0044 at -3.48</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0584 at -121.41</t>
+          <t>1.0423 at -122.75</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.9918 at 117.56</t>
+          <t>1.0175 at 117.05</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.0116 at -4.90</t>
+          <t>1.0015 at -3.48</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.9915 at 117.55</t>
+          <t>1.0188 at 117.01</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.9920 at 117.52</t>
+          <t>1.0202 at 116.93</t>
         </is>
       </c>
     </row>
@@ -621,17 +621,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.0050 at -4.93</t>
+          <t>1.0055 at -3.58</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0598 at -121.52</t>
+          <t>1.0436 at -122.84</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.9889 at 117.62</t>
+          <t>1.0190 at 116.97</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1.0121 at -4.75</t>
+          <t>1.0044 at -3.48</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0584 at -121.41</t>
+          <t>1.0423 at -122.75</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.9918 at 117.56</t>
+          <t>1.0175 at 117.05</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1.0082 at -5.18</t>
+          <t>0.9959 at -3.41</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">

</xml_diff>

<commit_message>
IEEE 13-bus test case
</commit_message>
<xml_diff>
--- a/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
+++ b/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0389 at -121.85</t>
+          <t>1.0328 at -121.90</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.0140 at 117.90</t>
+          <t>1.0154 at 117.86</t>
         </is>
       </c>
     </row>
@@ -506,12 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0372 at -121.92</t>
+          <t>1.0311 at -121.98</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.0119 at 117.95</t>
+          <t>1.0134 at 117.90</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.0209 at -2.49</t>
+          <t>1.0180 at -2.55</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0419 at -121.72</t>
+          <t>1.0401 at -121.77</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.0173 at 117.83</t>
+          <t>1.0148 at 117.83</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.0202 at -2.51</t>
+          <t>0.9940 at -3.23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0414 at -121.73</t>
+          <t>1.0218 at -122.22</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.0168 at 117.82</t>
+          <t>0.9960 at 117.35</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.0044 at -3.48</t>
+          <t>0.9814 at -5.62</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0423 at -122.75</t>
+          <t>1.0592 at -122.68</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.0175 at 117.05</t>
+          <t>0.9869 at 117.30</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.0015 at -3.48</t>
+          <t>0.9779 at -5.67</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.0188 at 117.01</t>
+          <t>0.9887 at 117.47</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.0202 at 116.93</t>
+          <t>0.9905 at 117.59</t>
         </is>
       </c>
     </row>
@@ -621,17 +621,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.0055 at -3.58</t>
+          <t>0.9748 at -5.87</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0436 at -122.84</t>
+          <t>1.0616 at -122.86</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.0190 at 116.97</t>
+          <t>0.9852 at 117.31</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1.0044 at -3.48</t>
+          <t>0.9814 at -5.62</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0423 at -122.75</t>
+          <t>1.0592 at -122.68</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.0175 at 117.05</t>
+          <t>0.9869 at 117.30</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.9959 at -3.41</t>
+          <t>0.9724 at -5.59</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">

</xml_diff>

<commit_message>
IEEE 13-bus test case OK
</commit_message>
<xml_diff>
--- a/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
+++ b/src/trunk/unbalanced_pf/tensiones_trifasicas.xlsx
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.0000 at 0.00</t>
+          <t>1.0210 at -2.49</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1.0000 at -120.00</t>
+          <t>1.0420 at -121.72</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0000 at 120.00</t>
+          <t>1.0174 at 117.83</t>
         </is>
       </c>
     </row>
@@ -486,12 +486,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9907 at -120.19</t>
+          <t>1.0328 at -121.90</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.9982 at 120.02</t>
+          <t>1.0154 at 117.86</t>
         </is>
       </c>
     </row>
@@ -506,12 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9890 at -120.26</t>
+          <t>1.0311 at -121.98</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.9962 at 120.07</t>
+          <t>1.0134 at 117.90</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.9969 at -0.07</t>
+          <t>1.0180 at -2.55</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9980 at -120.05</t>
+          <t>1.0401 at -121.77</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.9973 at 119.99</t>
+          <t>1.0148 at 117.83</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.9724 at -0.77</t>
+          <t>0.9940 at -3.23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9788 at -120.55</t>
+          <t>1.0218 at -122.22</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.9782 at 119.50</t>
+          <t>0.9960 at 117.35</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.9641 at -3.02</t>
+          <t>0.9900 at -5.30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0154 at -121.01</t>
+          <t>1.0529 at -122.34</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.9686 at 119.75</t>
+          <t>0.9777 at 116.03</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.9606 at -3.07</t>
+          <t>0.9881 at -5.32</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.9705 at 119.92</t>
+          <t>0.9757 at 115.93</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.9724 at 120.05</t>
+          <t>0.9737 at 115.78</t>
         </is>
       </c>
     </row>
@@ -621,17 +621,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.9574 at -3.28</t>
+          <t>0.9835 at -5.55</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0177 at -121.19</t>
+          <t>1.0553 at -122.52</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.9667 at 119.76</t>
+          <t>0.9758 at 116.04</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.9641 at -3.02</t>
+          <t>0.9900 at -5.30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0154 at -121.01</t>
+          <t>1.0529 at -122.34</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.9686 at 119.75</t>
+          <t>0.9777 at 116.03</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.9552 at -2.99</t>
+          <t>0.9825 at -5.25</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">

</xml_diff>